<commit_message>
ano 17 et po 17 correct
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RSA ANO 17.xlsx
+++ b/formats/excel/Formats RSA ANO 17.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$106</definedName>
+  </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217">
   <si>
     <t>libelle</t>
   </si>
@@ -29,6 +32,9 @@
   </si>
   <si>
     <t>nom</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
   <si>
     <t>N° FINESS e-PMSI</t>
@@ -669,10 +675,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -721,15 +727,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -744,6 +742,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -753,7 +772,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -767,11 +801,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -782,8 +815,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -797,22 +831,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -826,37 +847,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,7 +895,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -901,7 +943,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,37 +1033,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -955,115 +1063,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1137,7 +1137,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1146,7 +1161,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1162,6 +1177,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1185,174 +1215,144 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1754,9 +1754,9 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22:A52"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1765,7 +1765,7 @@
     <col min="5" max="5" width="14.8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1781,10 +1781,13 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" ht="15" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3">
         <v>9</v>
@@ -1796,15 +1799,15 @@
         <v>9</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -1816,15 +1819,15 @@
         <v>12</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1836,15 +1839,15 @@
         <v>15</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -1856,15 +1859,15 @@
         <v>17</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -1876,15 +1879,15 @@
         <v>21</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -1896,15 +1899,15 @@
         <v>22</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -1916,15 +1919,15 @@
         <v>23</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
@@ -1936,15 +1939,15 @@
         <v>24</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -1956,15 +1959,15 @@
         <v>25</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
@@ -1976,15 +1979,15 @@
         <v>26</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -1996,15 +1999,15 @@
         <v>27</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
@@ -2016,15 +2019,15 @@
         <v>28</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:6">
       <c r="A14" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -2036,15 +2039,15 @@
         <v>29</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:6">
       <c r="A15" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -2056,15 +2059,15 @@
         <v>30</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3">
         <v>17</v>
@@ -2076,15 +2079,15 @@
         <v>47</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:6">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="10">
         <v>17</v>
@@ -2096,15 +2099,15 @@
         <v>64</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3">
         <v>5</v>
@@ -2116,15 +2119,15 @@
         <v>69</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="3">
         <v>10</v>
@@ -2136,15 +2139,15 @@
         <v>79</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:6">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="3">
         <v>8</v>
@@ -2156,15 +2159,15 @@
         <v>87</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:6">
       <c r="A21" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="3">
         <v>8</v>
@@ -2176,15 +2179,15 @@
         <v>95</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="3">
         <v>1</v>
@@ -2196,15 +2199,15 @@
         <v>96</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:6">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
@@ -2216,15 +2219,15 @@
         <v>97</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -2236,15 +2239,15 @@
         <v>98</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -2256,15 +2259,15 @@
         <v>99</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -2276,15 +2279,15 @@
         <v>100</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -2296,15 +2299,15 @@
         <v>101</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -2316,15 +2319,15 @@
         <v>102</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
@@ -2336,15 +2339,15 @@
         <v>103</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
@@ -2356,15 +2359,15 @@
         <v>104</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" s="4">
         <v>1</v>
@@ -2376,15 +2379,15 @@
         <v>105</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
@@ -2396,15 +2399,15 @@
         <v>106</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
@@ -2416,15 +2419,15 @@
         <v>107</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
@@ -2436,15 +2439,15 @@
         <v>108</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
@@ -2456,15 +2459,15 @@
         <v>109</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
@@ -2476,15 +2479,15 @@
         <v>110</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
@@ -2496,15 +2499,15 @@
         <v>111</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:6">
       <c r="A38" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
@@ -2516,15 +2519,15 @@
         <v>112</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:6">
       <c r="A39" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
@@ -2536,15 +2539,15 @@
         <v>113</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:6">
       <c r="A40" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="4">
         <v>1</v>
@@ -2556,15 +2559,15 @@
         <v>114</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:6">
       <c r="A41" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B41" s="4">
         <v>1</v>
@@ -2576,15 +2579,15 @@
         <v>115</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:6">
       <c r="A42" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -2596,15 +2599,15 @@
         <v>116</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -2616,15 +2619,15 @@
         <v>117</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:6">
       <c r="A44" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -2636,15 +2639,15 @@
         <v>118</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:6">
       <c r="A45" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -2656,15 +2659,15 @@
         <v>119</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:6">
       <c r="A46" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -2676,15 +2679,15 @@
         <v>120</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:6">
       <c r="A47" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -2696,15 +2699,15 @@
         <v>121</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:6">
       <c r="A48" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -2716,15 +2719,15 @@
         <v>122</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:6">
       <c r="A49" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
@@ -2736,15 +2739,15 @@
         <v>123</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:6">
       <c r="A50" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -2756,15 +2759,15 @@
         <v>124</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:6">
       <c r="A51" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B51" s="14">
         <v>1</v>
@@ -2776,15 +2779,15 @@
         <v>125</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:6">
       <c r="A52" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
@@ -2796,15 +2799,15 @@
         <v>126</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:6">
       <c r="A53" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B53" s="17">
         <v>1</v>
@@ -2816,15 +2819,15 @@
         <v>127</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:6">
       <c r="A54" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B54" s="17">
         <v>1</v>
@@ -2836,15 +2839,15 @@
         <v>128</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:6">
       <c r="A55" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B55" s="17">
         <v>1</v>
@@ -2856,15 +2859,15 @@
         <v>129</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:6">
       <c r="A56" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B56" s="17">
         <v>1</v>
@@ -2876,15 +2879,15 @@
         <v>130</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:6">
       <c r="A57" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B57" s="17">
         <v>1</v>
@@ -2896,15 +2899,15 @@
         <v>131</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:6">
       <c r="A58" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58" s="17">
         <v>1</v>
@@ -2916,15 +2919,15 @@
         <v>132</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:6">
       <c r="A59" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B59" s="17">
         <v>1</v>
@@ -2936,15 +2939,15 @@
         <v>133</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:6">
       <c r="A60" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B60" s="17">
         <v>1</v>
@@ -2956,15 +2959,15 @@
         <v>134</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:6">
       <c r="A61" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B61" s="17">
         <v>1</v>
@@ -2976,15 +2979,15 @@
         <v>135</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:6">
       <c r="A62" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B62" s="17">
         <v>1</v>
@@ -2996,15 +2999,15 @@
         <v>136</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B63" s="4">
         <v>2</v>
@@ -3016,15 +3019,15 @@
         <v>138</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B64" s="4">
         <v>2</v>
@@ -3036,15 +3039,15 @@
         <v>140</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:6">
       <c r="A65" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>
@@ -3056,15 +3059,15 @@
         <v>141</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:6">
       <c r="A66" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B66" s="21">
         <v>1</v>
@@ -3076,15 +3079,15 @@
         <v>142</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:6">
       <c r="A67" s="20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B67" s="20">
         <v>2</v>
@@ -3096,15 +3099,15 @@
         <v>144</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" ht="15" spans="1:6">
       <c r="A68" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B68" s="20">
         <v>2</v>
@@ -3116,15 +3119,15 @@
         <v>146</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:6">
       <c r="A69" s="20" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B69" s="20">
         <v>1</v>
@@ -3136,15 +3139,15 @@
         <v>147</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B70" s="3">
         <v>1</v>
@@ -3156,15 +3159,15 @@
         <v>148</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" ht="15" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -3176,15 +3179,15 @@
         <v>149</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" ht="15" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B72" s="4">
         <v>4</v>
@@ -3196,15 +3199,15 @@
         <v>153</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" ht="15" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B73" s="4">
         <v>10</v>
@@ -3216,15 +3219,15 @@
         <v>163</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" ht="15" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B74" s="4">
         <v>10</v>
@@ -3236,15 +3239,15 @@
         <v>173</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" ht="15" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B75" s="4">
         <v>10</v>
@@ -3256,15 +3259,15 @@
         <v>183</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" ht="15" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B76" s="4">
         <v>4</v>
@@ -3276,15 +3279,15 @@
         <v>187</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" ht="15" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B77" s="4">
         <v>10</v>
@@ -3296,15 +3299,15 @@
         <v>197</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" ht="15" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B78" s="4">
         <v>5</v>
@@ -3316,15 +3319,15 @@
         <v>202</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" ht="15" spans="1:6">
       <c r="A79" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B79" s="4">
         <v>1</v>
@@ -3336,15 +3339,15 @@
         <v>203</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" ht="15" spans="1:6">
       <c r="A80" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B80" s="23">
         <v>32</v>
@@ -3356,15 +3359,15 @@
         <v>235</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" ht="15" spans="1:6">
       <c r="A81" s="25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B81" s="11">
         <v>32</v>
@@ -3376,13 +3379,15 @@
         <v>267</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="F81" s="19"/>
+        <v>168</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="82" ht="15" spans="1:6">
       <c r="A82" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B82" s="4">
         <v>1</v>
@@ -3394,15 +3399,15 @@
         <v>268</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" ht="15" spans="1:6">
       <c r="A83" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B83" s="4">
         <v>1</v>
@@ -3414,15 +3419,15 @@
         <v>269</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" ht="15" spans="1:6">
       <c r="A84" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B84" s="4">
         <v>8</v>
@@ -3434,15 +3439,15 @@
         <v>277</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" ht="15" spans="1:6">
       <c r="A85" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B85" s="4">
         <v>10</v>
@@ -3454,15 +3459,15 @@
         <v>287</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" ht="15" spans="1:6">
       <c r="A86" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B86" s="4">
         <v>1</v>
@@ -3474,15 +3479,15 @@
         <v>288</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" ht="15" spans="1:6">
       <c r="A87" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B87" s="4">
         <v>6</v>
@@ -3494,16 +3499,14 @@
         <v>294</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" ht="15" spans="1:6">
-      <c r="A88" s="27" t="s">
-        <v>180</v>
-      </c>
+      <c r="A88" s="27"/>
       <c r="B88" s="4">
         <v>3</v>
       </c>
@@ -3514,15 +3517,15 @@
         <v>297</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" ht="15" spans="1:6">
       <c r="A89" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B89" s="4">
         <v>1</v>
@@ -3534,15 +3537,15 @@
         <v>298</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" ht="15" spans="1:6">
       <c r="A90" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B90" s="4">
         <v>3</v>
@@ -3554,15 +3557,15 @@
         <v>301</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" ht="15" spans="1:6">
       <c r="A91" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="4">
         <v>3</v>
@@ -3574,15 +3577,15 @@
         <v>304</v>
       </c>
       <c r="E91" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" ht="15" spans="1:6">
       <c r="A92" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B92" s="4">
         <v>4</v>
@@ -3594,15 +3597,15 @@
         <v>308</v>
       </c>
       <c r="E92" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" ht="15" spans="1:6">
       <c r="A93" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B93" s="4">
         <v>1</v>
@@ -3614,15 +3617,15 @@
         <v>309</v>
       </c>
       <c r="E93" s="18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" ht="15" spans="1:6">
       <c r="A94" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B94" s="4">
         <v>9</v>
@@ -3634,15 +3637,15 @@
         <v>318</v>
       </c>
       <c r="E94" s="18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95" ht="15" spans="1:6">
       <c r="A95" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B95" s="4">
         <v>10</v>
@@ -3654,15 +3657,15 @@
         <v>328</v>
       </c>
       <c r="E95" s="18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="25" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B96" s="11">
         <v>1</v>
@@ -3674,15 +3677,15 @@
         <v>329</v>
       </c>
       <c r="E96" s="18" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F96" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B97" s="11">
         <v>8</v>
@@ -3694,15 +3697,15 @@
         <v>337</v>
       </c>
       <c r="E97" s="18" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F97" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="25" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B98" s="11">
         <v>8</v>
@@ -3714,15 +3717,15 @@
         <v>345</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F98" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="25" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B99" s="11">
         <v>3</v>
@@ -3734,15 +3737,15 @@
         <v>348</v>
       </c>
       <c r="E99" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F99" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="25" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B100" s="11">
         <v>3</v>
@@ -3754,15 +3757,15 @@
         <v>351</v>
       </c>
       <c r="E100" s="18" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F100" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="25" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B101" s="11">
         <v>1</v>
@@ -3774,15 +3777,15 @@
         <v>352</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F101" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B102" s="11">
         <v>8</v>
@@ -3794,15 +3797,15 @@
         <v>360</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F102" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="25" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B103" s="11">
         <v>8</v>
@@ -3814,16 +3817,14 @@
         <v>368</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F103" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="25" t="s">
-        <v>180</v>
-      </c>
+      <c r="A104" s="25"/>
       <c r="B104" s="11">
         <v>18</v>
       </c>
@@ -3834,15 +3835,15 @@
         <v>386</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F104" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="25" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B105" s="11">
         <v>64</v>
@@ -3854,15 +3855,15 @@
         <v>450</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F105" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="25" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B106" s="11">
         <v>344</v>
@@ -3874,13 +3875,14 @@
         <v>794</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F106" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F106"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>